<commit_message>
Mental Health updates and reconfiguration
Added additional scalar for MH, reconfigured package
</commit_message>
<xml_diff>
--- a/createSystemData/data_tests/testResults_fredi_general.xlsx
+++ b/createSystemData/data_tests/testResults_fredi_general.xlsx
@@ -522,10 +522,10 @@
         <v>18</v>
       </c>
       <c r="D2" t="n">
-        <v>202176</v>
+        <v>213840</v>
       </c>
       <c r="E2" t="n">
-        <v>202176</v>
+        <v>213840</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -551,10 +551,10 @@
         <v>18</v>
       </c>
       <c r="D3" t="n">
-        <v>202176</v>
+        <v>213840</v>
       </c>
       <c r="E3" t="n">
-        <v>202176</v>
+        <v>213840</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>

</xml_diff>